<commit_message>
Add support for random choice between loss functions on a per-batch basis
</commit_message>
<xml_diff>
--- a/analysis/correlation_across_heldout_sets.xlsx
+++ b/analysis/correlation_across_heldout_sets.xlsx
@@ -14,7 +14,6 @@
     <sheet name="150-ep-all" sheetId="9" r:id="rId5"/>
   </sheets>
   <calcPr calcId="145621"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -1884,11 +1883,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="79304960"/>
-        <c:axId val="79323520"/>
+        <c:axId val="67966464"/>
+        <c:axId val="121431552"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="79304960"/>
+        <c:axId val="67966464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1921,12 +1920,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="79323520"/>
+        <c:crossAx val="121431552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="79323520"/>
+        <c:axId val="121431552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1960,7 +1959,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="79304960"/>
+        <c:crossAx val="67966464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2285,11 +2284,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="81202176"/>
-        <c:axId val="81216640"/>
+        <c:axId val="101624064"/>
+        <c:axId val="101630336"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="81202176"/>
+        <c:axId val="101624064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2317,12 +2316,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="81216640"/>
+        <c:crossAx val="101630336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="81216640"/>
+        <c:axId val="101630336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2351,7 +2350,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="81202176"/>
+        <c:crossAx val="101624064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2406,7 +2405,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -3510,11 +3508,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="83494016"/>
-        <c:axId val="83495936"/>
+        <c:axId val="101769600"/>
+        <c:axId val="101771520"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="83494016"/>
+        <c:axId val="101769600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3541,19 +3539,18 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="83495936"/>
+        <c:crossAx val="101771520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="83495936"/>
+        <c:axId val="101771520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3581,21 +3578,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="83494016"/>
+        <c:crossAx val="101769600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -4663,11 +4658,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="83552896"/>
-        <c:axId val="83555072"/>
+        <c:axId val="77010816"/>
+        <c:axId val="77033472"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="83552896"/>
+        <c:axId val="77010816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4696,12 +4691,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="83555072"/>
+        <c:crossAx val="77033472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="83555072"/>
+        <c:axId val="77033472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4736,7 +4731,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="83552896"/>
+        <c:crossAx val="77010816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5758,11 +5753,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="84107648"/>
-        <c:axId val="84109568"/>
+        <c:axId val="77053312"/>
+        <c:axId val="77055488"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="84107648"/>
+        <c:axId val="77053312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5791,12 +5786,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="84109568"/>
+        <c:crossAx val="77055488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="84109568"/>
+        <c:axId val="77055488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5826,7 +5821,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="84107648"/>
+        <c:crossAx val="77053312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5873,7 +5868,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -7476,11 +7470,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="84566016"/>
-        <c:axId val="84567936"/>
+        <c:axId val="83461248"/>
+        <c:axId val="83463168"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="84566016"/>
+        <c:axId val="83461248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7502,19 +7496,18 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="84567936"/>
+        <c:crossAx val="83463168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="84567936"/>
+        <c:axId val="83463168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7537,21 +7530,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="84566016"/>
+        <c:crossAx val="83461248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -7596,7 +7587,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -9130,11 +9120,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="84605184"/>
-        <c:axId val="84287488"/>
+        <c:axId val="83488128"/>
+        <c:axId val="83530880"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="84605184"/>
+        <c:axId val="83488128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9144,12 +9134,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="84287488"/>
+        <c:crossAx val="83530880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="84287488"/>
+        <c:axId val="83530880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9172,14 +9162,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="84605184"/>
+        <c:crossAx val="83488128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -9226,7 +9215,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -10813,11 +10801,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="116327552"/>
-        <c:axId val="110816640"/>
+        <c:axId val="101610240"/>
+        <c:axId val="101612160"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="116327552"/>
+        <c:axId val="101610240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10839,19 +10827,18 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="110816640"/>
+        <c:crossAx val="101612160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="110816640"/>
+        <c:axId val="101612160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10874,21 +10861,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="116327552"/>
+        <c:crossAx val="101610240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -13469,8 +13454,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD148"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H37" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="V30" sqref="V30"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>